<commit_message>
add test cases and documentation
</commit_message>
<xml_diff>
--- a/src/tests/option-ec.test-cases.xlsx
+++ b/src/tests/option-ec.test-cases.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20077A40-7B8F-C542-8051-73C1E2AFACA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A9862F-FA6E-E044-BB96-53E4A9D689C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="2920" windowWidth="40760" windowHeight="23140" activeTab="1" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="9520" yWindow="2920" windowWidth="40760" windowHeight="23140" activeTab="2" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="44" r:id="rId1"/>
     <sheet name="ec01" sheetId="2" r:id="rId2"/>
+    <sheet name="ec02" sheetId="45" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="105">
   <si>
     <t>case</t>
     <phoneticPr fontId="1"/>
@@ -627,6 +628,29 @@
       <t>ゾウカ</t>
     </rPh>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>4-room</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30-renewable</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>march</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>december</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ec02</t>
+  </si>
+  <si>
+    <t>ec02</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1098,6 +1122,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="12" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1107,14 +1139,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="パーセント" xfId="1" builtinId="5"/>
@@ -1438,10 +1462,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1707,6 +1731,240 @@
       </c>
       <c r="F14" s="2"/>
     </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="19">
+        <v>5</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1">
+        <v>750</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="1">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1">
+        <v>200</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1720,7 +1978,7 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1775,11 +2033,11 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -1907,7 +2165,7 @@
       <c r="C5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="42">
         <v>22.122598967509795</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -1931,7 +2189,7 @@
       <c r="K5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="43" t="s">
         <v>91</v>
       </c>
       <c r="M5" s="34">
@@ -2295,10 +2553,10 @@
       <c r="K14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L14" s="47" t="s">
+      <c r="L14" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="M14" s="48">
+      <c r="M14" s="45">
         <v>0.27166666666666667</v>
       </c>
       <c r="N14" s="7"/>
@@ -2684,4 +2942,977 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D055DF44-5F25-334D-9007-D260A9CDBBD9}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="66.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="37">
+        <v>9.8661482141591677</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="39"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="38">
+        <v>2.1338517858408315</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="27"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
+    </row>
+    <row r="4" spans="1:14" ht="21" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="38">
+        <v>1.9614220396155515</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="42">
+        <v>18.775467972643419</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" s="34">
+        <v>-7.7669902912621394E-2</v>
+      </c>
+      <c r="N5" s="35"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="31">
+        <v>1533.7634058264055</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="M7" s="34">
+        <v>0.60378510378510375</v>
+      </c>
+      <c r="N7" s="35"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="31">
+        <v>309.00655477412886</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="34">
+        <v>0.63325991189427322</v>
+      </c>
+      <c r="N8" s="35"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="M9" s="34">
+        <v>0.22822085889570551</v>
+      </c>
+      <c r="N9" s="35"/>
+    </row>
+    <row r="10" spans="1:14" ht="21" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="32">
+        <v>3.333027350494596</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="34">
+        <v>0.93919766762846524</v>
+      </c>
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="22">
+        <v>103.55050000000001</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="30"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="13"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="23">
+        <v>0.93069899951528912</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="36"/>
+      <c r="M12" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="24">
+        <v>3.4180806918018205</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="36"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0.54238644061711094</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="L14" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" s="45">
+        <v>0.27166666666666667</v>
+      </c>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="24">
+        <v>1.3782452040258706</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" s="36"/>
+      <c r="M15" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0.53349389026516225</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16" s="36"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="24">
+        <v>0.3105447626180039</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="27"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="24">
+        <v>0.32756490664331728</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="29"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="24">
+        <v>0.28008110814182374</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="29"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="24">
+        <v>3.7319211581766772E-2</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="29"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="25">
+        <v>0.58446220328405674</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="30"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="D2:D4 D6:D11">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BED6EC9F-6597-0444-B2AC-F0F0304537A9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{98997031-52F7-D748-A7CC-0769C0CD68AB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D15 D17:D21">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A3F0D6DF-5DDB-034E-83AD-B25DA2128D0A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C09D1E49-8F17-B94D-8BC4-4FE605C69B12}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BED6EC9F-6597-0444-B2AC-F0F0304537A9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D2:D4 D6:D11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{98997031-52F7-D748-A7CC-0769C0CD68AB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A3F0D6DF-5DDB-034E-83AD-B25DA2128D0A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D12:D15 D17:D21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C09D1E49-8F17-B94D-8BC4-4FE605C69B12}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D16</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>